<commit_message>
Refactor user authentication views and improve styling
</commit_message>
<xml_diff>
--- a/public/assets/templates/template_level.xlsx
+++ b/public/assets/templates/template_level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Instalasi\Laragon\laragon\www\POS_2025\public\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E6581D-037A-4BB3-96FB-49E270482593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67D89C7-696B-47A3-A412-4C9275E334D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>level_kode</t>
   </si>
   <si>
     <t>level_nama</t>
+  </si>
+  <si>
+    <t>MHS</t>
+  </si>
+  <si>
+    <t>Mahasiswa</t>
+  </si>
+  <si>
+    <t>DSN</t>
+  </si>
+  <si>
+    <t>Dosen</t>
   </si>
 </sst>
 </file>
@@ -290,10 +302,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -306,6 +318,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>